<commit_message>
added US data to nonuc scenario
Former-commit-id: f0a0d577a6a1496f361f13b2655b2e068d2d35a5
Former-commit-id: 149443d279b80526856c3b2089396cfa4e1a7b74
</commit_message>
<xml_diff>
--- a/data/japan_costs/fossil-ccs-nuc.xlsx
+++ b/data/japan_costs/fossil-ccs-nuc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arfc\Documents\GitHub\i2cner\data\japan_costs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alley cat\Documents\GitHub\i2cner\data\japan_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F7AE7E-8228-4B4E-A466-F2238D8D9CFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84393D9D-A509-46B2-85B5-647328347890}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="2970" windowWidth="19755" windowHeight="10155" xr2:uid="{558254C2-F576-4D72-B799-A1AA36A7D720}"/>
+    <workbookView minimized="1" xWindow="3300" yWindow="3300" windowWidth="21600" windowHeight="11325" xr2:uid="{558254C2-F576-4D72-B799-A1AA36A7D720}"/>
   </bookViews>
   <sheets>
     <sheet name="Coal" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>